<commit_message>
Splitting Tree tests S-method results of some experiments
</commit_message>
<xml_diff>
--- a/data/experiments/resultsTesting.xlsx
+++ b/data/experiments/resultsTesting.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="10320" windowHeight="8160" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="10320" windowHeight="8160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="resultsTesting" sheetId="1" r:id="rId1"/>
     <sheet name="resultsTesting (2)" sheetId="2" r:id="rId2"/>
     <sheet name="resultsTesting2304" sheetId="3" r:id="rId3"/>
     <sheet name="resultsTesting2504" sheetId="4" r:id="rId4"/>
+    <sheet name="170526-S" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="34">
   <si>
     <t>Correct/IndistMachines</t>
   </si>
@@ -89,6 +90,36 @@
   </si>
   <si>
     <t>Mealy_R2_turnstile.fsm</t>
+  </si>
+  <si>
+    <t>PDS-method</t>
+  </si>
+  <si>
+    <t>ADS-method</t>
+  </si>
+  <si>
+    <t>SVS-method</t>
+  </si>
+  <si>
+    <t>W-method</t>
+  </si>
+  <si>
+    <t>Wp-method</t>
+  </si>
+  <si>
+    <t>HSI-method</t>
+  </si>
+  <si>
+    <t>S-method</t>
+  </si>
+  <si>
+    <t>Mra-method</t>
+  </si>
+  <si>
+    <t>Mrg-method</t>
+  </si>
+  <si>
+    <t>DFA_R664_pots2.fsm</t>
   </si>
 </sst>
 </file>
@@ -3983,7 +4014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -9255,4 +9286,3873 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M95"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>241</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>241</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1.0020000000000001E-3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>241</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>56359</v>
+      </c>
+      <c r="H4">
+        <v>2427143</v>
+      </c>
+      <c r="I4">
+        <v>1.1247450000000001</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>241</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>47250</v>
+      </c>
+      <c r="H5">
+        <v>1557872</v>
+      </c>
+      <c r="I5">
+        <v>0.61840899999999999</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>241</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>5913</v>
+      </c>
+      <c r="H6">
+        <v>192891</v>
+      </c>
+      <c r="I6">
+        <v>0.37424800000000003</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>241</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>7467</v>
+      </c>
+      <c r="H7">
+        <v>245826</v>
+      </c>
+      <c r="I7">
+        <v>0.11808</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>241</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>7139</v>
+      </c>
+      <c r="H8">
+        <v>241853</v>
+      </c>
+      <c r="I8">
+        <v>0.10506799999999999</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>241</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>6516</v>
+      </c>
+      <c r="H9">
+        <v>223588</v>
+      </c>
+      <c r="I9">
+        <v>7.8052999999999997E-2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="M9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>241</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>5909</v>
+      </c>
+      <c r="H10">
+        <v>195007</v>
+      </c>
+      <c r="I10">
+        <v>0.128085</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>241</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>5955</v>
+      </c>
+      <c r="H11">
+        <v>207013</v>
+      </c>
+      <c r="I11">
+        <v>6.4922950000000004</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11">
+        <v>9</v>
+      </c>
+      <c r="M11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>241</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>241</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13">
+        <v>11</v>
+      </c>
+      <c r="M13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>241</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>241</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1.0009999999999999E-3</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>241</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>841616</v>
+      </c>
+      <c r="H16">
+        <v>37958456</v>
+      </c>
+      <c r="I16">
+        <v>13.036626</v>
+      </c>
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>241</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>708750</v>
+      </c>
+      <c r="H17">
+        <v>24785580</v>
+      </c>
+      <c r="I17">
+        <v>7.2247810000000001</v>
+      </c>
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="M17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>241</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>56967</v>
+      </c>
+      <c r="H18">
+        <v>1932150</v>
+      </c>
+      <c r="I18">
+        <v>0.99165599999999998</v>
+      </c>
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="M18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>241</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>61398</v>
+      </c>
+      <c r="H19">
+        <v>2081596</v>
+      </c>
+      <c r="I19">
+        <v>0.60440099999999997</v>
+      </c>
+      <c r="J19" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" t="s">
+        <v>29</v>
+      </c>
+      <c r="L19">
+        <v>5</v>
+      </c>
+      <c r="M19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>241</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>58590</v>
+      </c>
+      <c r="H20">
+        <v>2007944</v>
+      </c>
+      <c r="I20">
+        <v>0.484321</v>
+      </c>
+      <c r="J20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20">
+        <v>6</v>
+      </c>
+      <c r="M20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>241</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>47513</v>
+      </c>
+      <c r="H21">
+        <v>1634399</v>
+      </c>
+      <c r="I21">
+        <v>0.44529299999999999</v>
+      </c>
+      <c r="J21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21">
+        <v>7</v>
+      </c>
+      <c r="M21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>241</v>
+      </c>
+      <c r="D22">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>56812</v>
+      </c>
+      <c r="H22">
+        <v>1929454</v>
+      </c>
+      <c r="I22">
+        <v>0.78251899999999996</v>
+      </c>
+      <c r="J22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22">
+        <v>8</v>
+      </c>
+      <c r="M22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>241</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>57722</v>
+      </c>
+      <c r="H23">
+        <v>2003094</v>
+      </c>
+      <c r="I23">
+        <v>57.096783000000002</v>
+      </c>
+      <c r="J23" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23">
+        <v>9</v>
+      </c>
+      <c r="M23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>241</v>
+      </c>
+      <c r="D24">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24">
+        <v>10</v>
+      </c>
+      <c r="M24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>241</v>
+      </c>
+      <c r="D25">
+        <v>15</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" t="s">
+        <v>32</v>
+      </c>
+      <c r="L25">
+        <v>11</v>
+      </c>
+      <c r="M25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>50</v>
+      </c>
+      <c r="D26">
+        <v>18</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" t="s">
+        <v>24</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>50</v>
+      </c>
+      <c r="D27">
+        <v>18</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>50</v>
+      </c>
+      <c r="D28">
+        <v>18</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>2308</v>
+      </c>
+      <c r="H28">
+        <v>36834</v>
+      </c>
+      <c r="I28">
+        <v>1.9012000000000001E-2</v>
+      </c>
+      <c r="J28" t="s">
+        <v>13</v>
+      </c>
+      <c r="K28" t="s">
+        <v>26</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>50</v>
+      </c>
+      <c r="D29">
+        <v>18</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>13616</v>
+      </c>
+      <c r="H29">
+        <v>205158</v>
+      </c>
+      <c r="I29">
+        <v>5.8039E-2</v>
+      </c>
+      <c r="J29" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" t="s">
+        <v>27</v>
+      </c>
+      <c r="L29">
+        <v>3</v>
+      </c>
+      <c r="M29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>50</v>
+      </c>
+      <c r="D30">
+        <v>18</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>967</v>
+      </c>
+      <c r="H30">
+        <v>13710</v>
+      </c>
+      <c r="I30">
+        <v>1.3008E-2</v>
+      </c>
+      <c r="J30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" t="s">
+        <v>28</v>
+      </c>
+      <c r="L30">
+        <v>4</v>
+      </c>
+      <c r="M30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>50</v>
+      </c>
+      <c r="D31">
+        <v>18</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1253</v>
+      </c>
+      <c r="H31">
+        <v>18331</v>
+      </c>
+      <c r="I31">
+        <v>6.0039999999999998E-3</v>
+      </c>
+      <c r="J31" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31" t="s">
+        <v>29</v>
+      </c>
+      <c r="L31">
+        <v>5</v>
+      </c>
+      <c r="M31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>50</v>
+      </c>
+      <c r="D32">
+        <v>18</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>992</v>
+      </c>
+      <c r="H32">
+        <v>14508</v>
+      </c>
+      <c r="I32">
+        <v>4.0029999999999996E-3</v>
+      </c>
+      <c r="J32" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32">
+        <v>6</v>
+      </c>
+      <c r="M32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>50</v>
+      </c>
+      <c r="D33">
+        <v>18</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>1177</v>
+      </c>
+      <c r="H33">
+        <v>18545</v>
+      </c>
+      <c r="I33">
+        <v>6.0039999999999998E-3</v>
+      </c>
+      <c r="J33" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33">
+        <v>7</v>
+      </c>
+      <c r="M33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>50</v>
+      </c>
+      <c r="D34">
+        <v>18</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>1030</v>
+      </c>
+      <c r="H34">
+        <v>14716</v>
+      </c>
+      <c r="I34">
+        <v>5.0039999999999998E-3</v>
+      </c>
+      <c r="J34" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34" t="s">
+        <v>17</v>
+      </c>
+      <c r="L34">
+        <v>8</v>
+      </c>
+      <c r="M34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>50</v>
+      </c>
+      <c r="D35">
+        <v>18</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>990</v>
+      </c>
+      <c r="H35">
+        <v>15344</v>
+      </c>
+      <c r="I35">
+        <v>5.6036999999999997E-2</v>
+      </c>
+      <c r="J35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" t="s">
+        <v>30</v>
+      </c>
+      <c r="L35">
+        <v>9</v>
+      </c>
+      <c r="M35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>50</v>
+      </c>
+      <c r="D36">
+        <v>18</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" t="s">
+        <v>31</v>
+      </c>
+      <c r="L36">
+        <v>10</v>
+      </c>
+      <c r="M36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>50</v>
+      </c>
+      <c r="D37">
+        <v>18</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" t="s">
+        <v>32</v>
+      </c>
+      <c r="L37">
+        <v>11</v>
+      </c>
+      <c r="M37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>50</v>
+      </c>
+      <c r="D38">
+        <v>18</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" t="s">
+        <v>24</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>18</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K39" t="s">
+        <v>25</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>50</v>
+      </c>
+      <c r="D40">
+        <v>18</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>40926</v>
+      </c>
+      <c r="H40">
+        <v>732996</v>
+      </c>
+      <c r="I40">
+        <v>0.20113400000000001</v>
+      </c>
+      <c r="J40" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L40">
+        <v>2</v>
+      </c>
+      <c r="M40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>50</v>
+      </c>
+      <c r="D41">
+        <v>18</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>245088</v>
+      </c>
+      <c r="H41">
+        <v>4183020</v>
+      </c>
+      <c r="I41">
+        <v>0.98765499999999995</v>
+      </c>
+      <c r="J41" t="s">
+        <v>13</v>
+      </c>
+      <c r="K41" t="s">
+        <v>27</v>
+      </c>
+      <c r="L41">
+        <v>3</v>
+      </c>
+      <c r="M41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>50</v>
+      </c>
+      <c r="D42">
+        <v>18</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>15546</v>
+      </c>
+      <c r="H42">
+        <v>248930</v>
+      </c>
+      <c r="I42">
+        <v>8.3055000000000004E-2</v>
+      </c>
+      <c r="J42" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42" t="s">
+        <v>28</v>
+      </c>
+      <c r="L42">
+        <v>4</v>
+      </c>
+      <c r="M42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>50</v>
+      </c>
+      <c r="D43">
+        <v>18</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>16091</v>
+      </c>
+      <c r="H43">
+        <v>258276</v>
+      </c>
+      <c r="I43">
+        <v>6.5043000000000004E-2</v>
+      </c>
+      <c r="J43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" t="s">
+        <v>29</v>
+      </c>
+      <c r="L43">
+        <v>5</v>
+      </c>
+      <c r="M43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>50</v>
+      </c>
+      <c r="D44">
+        <v>18</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>15504</v>
+      </c>
+      <c r="H44">
+        <v>248024</v>
+      </c>
+      <c r="I44">
+        <v>3.9025999999999998E-2</v>
+      </c>
+      <c r="J44" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44" t="s">
+        <v>14</v>
+      </c>
+      <c r="L44">
+        <v>6</v>
+      </c>
+      <c r="M44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>50</v>
+      </c>
+      <c r="D45">
+        <v>18</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>14892</v>
+      </c>
+      <c r="H45">
+        <v>244290</v>
+      </c>
+      <c r="I45">
+        <v>5.5037000000000003E-2</v>
+      </c>
+      <c r="J45" t="s">
+        <v>13</v>
+      </c>
+      <c r="K45" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45">
+        <v>7</v>
+      </c>
+      <c r="M45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>50</v>
+      </c>
+      <c r="D46">
+        <v>18</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>15213</v>
+      </c>
+      <c r="H46">
+        <v>247021</v>
+      </c>
+      <c r="I46">
+        <v>5.2033999999999997E-2</v>
+      </c>
+      <c r="J46" t="s">
+        <v>13</v>
+      </c>
+      <c r="K46" t="s">
+        <v>17</v>
+      </c>
+      <c r="L46">
+        <v>8</v>
+      </c>
+      <c r="M46" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>50</v>
+      </c>
+      <c r="D47">
+        <v>18</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>15295</v>
+      </c>
+      <c r="H47">
+        <v>249881</v>
+      </c>
+      <c r="I47">
+        <v>0.50633600000000001</v>
+      </c>
+      <c r="J47" t="s">
+        <v>13</v>
+      </c>
+      <c r="K47" t="s">
+        <v>30</v>
+      </c>
+      <c r="L47">
+        <v>9</v>
+      </c>
+      <c r="M47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>50</v>
+      </c>
+      <c r="D48">
+        <v>18</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48" t="s">
+        <v>13</v>
+      </c>
+      <c r="K48" t="s">
+        <v>31</v>
+      </c>
+      <c r="L48">
+        <v>10</v>
+      </c>
+      <c r="M48" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>50</v>
+      </c>
+      <c r="D49">
+        <v>18</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49" t="s">
+        <v>13</v>
+      </c>
+      <c r="K49" t="s">
+        <v>32</v>
+      </c>
+      <c r="L49">
+        <v>11</v>
+      </c>
+      <c r="M49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>664</v>
+      </c>
+      <c r="D50">
+        <v>32</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>1.0009999999999999E-3</v>
+      </c>
+      <c r="J50" t="s">
+        <v>13</v>
+      </c>
+      <c r="K50" t="s">
+        <v>24</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>664</v>
+      </c>
+      <c r="D51">
+        <v>32</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>1.003E-3</v>
+      </c>
+      <c r="J51" t="s">
+        <v>13</v>
+      </c>
+      <c r="K51" t="s">
+        <v>25</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>664</v>
+      </c>
+      <c r="D52">
+        <v>32</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>277071</v>
+      </c>
+      <c r="H52">
+        <v>7862586</v>
+      </c>
+      <c r="I52">
+        <v>9.5072930000000007</v>
+      </c>
+      <c r="J52" t="s">
+        <v>13</v>
+      </c>
+      <c r="K52" t="s">
+        <v>26</v>
+      </c>
+      <c r="L52">
+        <v>2</v>
+      </c>
+      <c r="M52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>664</v>
+      </c>
+      <c r="D53">
+        <v>32</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>1176923</v>
+      </c>
+      <c r="H53">
+        <v>27953748</v>
+      </c>
+      <c r="I53">
+        <v>20.301435000000001</v>
+      </c>
+      <c r="J53" t="s">
+        <v>13</v>
+      </c>
+      <c r="K53" t="s">
+        <v>27</v>
+      </c>
+      <c r="L53">
+        <v>3</v>
+      </c>
+      <c r="M53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>664</v>
+      </c>
+      <c r="D54">
+        <v>32</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>53414</v>
+      </c>
+      <c r="H54">
+        <v>1194887</v>
+      </c>
+      <c r="I54">
+        <v>3.2191290000000001</v>
+      </c>
+      <c r="J54" t="s">
+        <v>13</v>
+      </c>
+      <c r="K54" t="s">
+        <v>28</v>
+      </c>
+      <c r="L54">
+        <v>4</v>
+      </c>
+      <c r="M54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>664</v>
+      </c>
+      <c r="D55">
+        <v>32</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>66192</v>
+      </c>
+      <c r="H55">
+        <v>1460311</v>
+      </c>
+      <c r="I55">
+        <v>0.67244300000000001</v>
+      </c>
+      <c r="J55" t="s">
+        <v>13</v>
+      </c>
+      <c r="K55" t="s">
+        <v>29</v>
+      </c>
+      <c r="L55">
+        <v>5</v>
+      </c>
+      <c r="M55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56">
+        <v>664</v>
+      </c>
+      <c r="D56">
+        <v>32</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>42862</v>
+      </c>
+      <c r="H56">
+        <v>997744</v>
+      </c>
+      <c r="I56">
+        <v>1.967303</v>
+      </c>
+      <c r="J56" t="s">
+        <v>13</v>
+      </c>
+      <c r="K56" t="s">
+        <v>14</v>
+      </c>
+      <c r="L56">
+        <v>6</v>
+      </c>
+      <c r="M56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>664</v>
+      </c>
+      <c r="D57">
+        <v>32</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>62917</v>
+      </c>
+      <c r="H57">
+        <v>1466787</v>
+      </c>
+      <c r="I57">
+        <v>0.61640899999999998</v>
+      </c>
+      <c r="J57" t="s">
+        <v>13</v>
+      </c>
+      <c r="K57" t="s">
+        <v>16</v>
+      </c>
+      <c r="L57">
+        <v>7</v>
+      </c>
+      <c r="M57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>664</v>
+      </c>
+      <c r="D58">
+        <v>32</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>48813</v>
+      </c>
+      <c r="H58">
+        <v>1054123</v>
+      </c>
+      <c r="I58">
+        <v>2.9369420000000002</v>
+      </c>
+      <c r="J58" t="s">
+        <v>13</v>
+      </c>
+      <c r="K58" t="s">
+        <v>17</v>
+      </c>
+      <c r="L58">
+        <v>8</v>
+      </c>
+      <c r="M58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>14</v>
+      </c>
+      <c r="D60">
+        <v>14</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>197</v>
+      </c>
+      <c r="H60">
+        <v>2768</v>
+      </c>
+      <c r="I60">
+        <v>0.17011399999999999</v>
+      </c>
+      <c r="J60" t="s">
+        <v>13</v>
+      </c>
+      <c r="K60" t="s">
+        <v>24</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>14</v>
+      </c>
+      <c r="D61">
+        <v>14</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>196</v>
+      </c>
+      <c r="H61">
+        <v>1971</v>
+      </c>
+      <c r="I61">
+        <v>9.990000000000001E-4</v>
+      </c>
+      <c r="J61" t="s">
+        <v>13</v>
+      </c>
+      <c r="K61" t="s">
+        <v>25</v>
+      </c>
+      <c r="L61">
+        <v>1</v>
+      </c>
+      <c r="M61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>14</v>
+      </c>
+      <c r="D62">
+        <v>14</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>258</v>
+      </c>
+      <c r="H62">
+        <v>1494</v>
+      </c>
+      <c r="I62">
+        <v>2.802E-2</v>
+      </c>
+      <c r="J62" t="s">
+        <v>13</v>
+      </c>
+      <c r="K62" t="s">
+        <v>26</v>
+      </c>
+      <c r="L62">
+        <v>2</v>
+      </c>
+      <c r="M62" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>14</v>
+      </c>
+      <c r="D63">
+        <v>14</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>2196</v>
+      </c>
+      <c r="H63">
+        <v>11256</v>
+      </c>
+      <c r="I63">
+        <v>4.0029999999999996E-3</v>
+      </c>
+      <c r="J63" t="s">
+        <v>13</v>
+      </c>
+      <c r="K63" t="s">
+        <v>27</v>
+      </c>
+      <c r="L63">
+        <v>3</v>
+      </c>
+      <c r="M63" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>0</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>14</v>
+      </c>
+      <c r="D64">
+        <v>14</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>469</v>
+      </c>
+      <c r="H64">
+        <v>2552</v>
+      </c>
+      <c r="I64">
+        <v>2E-3</v>
+      </c>
+      <c r="J64" t="s">
+        <v>13</v>
+      </c>
+      <c r="K64" t="s">
+        <v>28</v>
+      </c>
+      <c r="L64">
+        <v>4</v>
+      </c>
+      <c r="M64" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65">
+        <v>14</v>
+      </c>
+      <c r="D65">
+        <v>14</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>1096</v>
+      </c>
+      <c r="H65">
+        <v>6058</v>
+      </c>
+      <c r="I65">
+        <v>2.0019999999999999E-3</v>
+      </c>
+      <c r="J65" t="s">
+        <v>13</v>
+      </c>
+      <c r="K65" t="s">
+        <v>29</v>
+      </c>
+      <c r="L65">
+        <v>5</v>
+      </c>
+      <c r="M65" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>0</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <v>14</v>
+      </c>
+      <c r="D66">
+        <v>14</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>745</v>
+      </c>
+      <c r="H66">
+        <v>4592</v>
+      </c>
+      <c r="I66">
+        <v>2.0010000000000002E-3</v>
+      </c>
+      <c r="J66" t="s">
+        <v>13</v>
+      </c>
+      <c r="K66" t="s">
+        <v>14</v>
+      </c>
+      <c r="L66">
+        <v>6</v>
+      </c>
+      <c r="M66" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>0</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67">
+        <v>14</v>
+      </c>
+      <c r="D67">
+        <v>14</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>211</v>
+      </c>
+      <c r="H67">
+        <v>2617</v>
+      </c>
+      <c r="I67">
+        <v>5.0049999999999999E-3</v>
+      </c>
+      <c r="J67" t="s">
+        <v>13</v>
+      </c>
+      <c r="K67" t="s">
+        <v>16</v>
+      </c>
+      <c r="L67">
+        <v>7</v>
+      </c>
+      <c r="M67" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>0</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>14</v>
+      </c>
+      <c r="D68">
+        <v>14</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>412</v>
+      </c>
+      <c r="H68">
+        <v>2738</v>
+      </c>
+      <c r="I68">
+        <v>4.0029999999999996E-3</v>
+      </c>
+      <c r="J68" t="s">
+        <v>13</v>
+      </c>
+      <c r="K68" t="s">
+        <v>17</v>
+      </c>
+      <c r="L68">
+        <v>8</v>
+      </c>
+      <c r="M68" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69">
+        <v>14</v>
+      </c>
+      <c r="D69">
+        <v>14</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>114</v>
+      </c>
+      <c r="H69">
+        <v>1514</v>
+      </c>
+      <c r="I69">
+        <v>2.8018000000000001E-2</v>
+      </c>
+      <c r="J69" t="s">
+        <v>13</v>
+      </c>
+      <c r="K69" t="s">
+        <v>30</v>
+      </c>
+      <c r="L69">
+        <v>9</v>
+      </c>
+      <c r="M69" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>0</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70">
+        <v>14</v>
+      </c>
+      <c r="D70">
+        <v>14</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>4</v>
+      </c>
+      <c r="H70">
+        <v>1455</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70" t="s">
+        <v>13</v>
+      </c>
+      <c r="K70" t="s">
+        <v>31</v>
+      </c>
+      <c r="L70">
+        <v>10</v>
+      </c>
+      <c r="M70" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>0</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71">
+        <v>14</v>
+      </c>
+      <c r="D71">
+        <v>14</v>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>5</v>
+      </c>
+      <c r="H71">
+        <v>1518</v>
+      </c>
+      <c r="I71">
+        <v>6.0060000000000001E-3</v>
+      </c>
+      <c r="J71" t="s">
+        <v>13</v>
+      </c>
+      <c r="K71" t="s">
+        <v>32</v>
+      </c>
+      <c r="L71">
+        <v>11</v>
+      </c>
+      <c r="M71" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72">
+        <v>14</v>
+      </c>
+      <c r="D72">
+        <v>14</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>2759</v>
+      </c>
+      <c r="H72">
+        <v>41520</v>
+      </c>
+      <c r="I72">
+        <v>0.18712500000000001</v>
+      </c>
+      <c r="J72" t="s">
+        <v>13</v>
+      </c>
+      <c r="K72" t="s">
+        <v>24</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>0</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73">
+        <v>14</v>
+      </c>
+      <c r="D73">
+        <v>14</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>2743</v>
+      </c>
+      <c r="H73">
+        <v>30604</v>
+      </c>
+      <c r="I73">
+        <v>1.2008E-2</v>
+      </c>
+      <c r="J73" t="s">
+        <v>13</v>
+      </c>
+      <c r="K73" t="s">
+        <v>25</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
+      <c r="M73" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>0</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <v>14</v>
+      </c>
+      <c r="D74">
+        <v>14</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74">
+        <v>3674</v>
+      </c>
+      <c r="H74">
+        <v>24868</v>
+      </c>
+      <c r="I74">
+        <v>3.5024E-2</v>
+      </c>
+      <c r="J74" t="s">
+        <v>13</v>
+      </c>
+      <c r="K74" t="s">
+        <v>26</v>
+      </c>
+      <c r="L74">
+        <v>2</v>
+      </c>
+      <c r="M74" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>0</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <v>14</v>
+      </c>
+      <c r="D75">
+        <v>14</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>30744</v>
+      </c>
+      <c r="H75">
+        <v>188328</v>
+      </c>
+      <c r="I75">
+        <v>5.9041999999999997E-2</v>
+      </c>
+      <c r="J75" t="s">
+        <v>13</v>
+      </c>
+      <c r="K75" t="s">
+        <v>27</v>
+      </c>
+      <c r="L75">
+        <v>3</v>
+      </c>
+      <c r="M75" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76">
+        <v>14</v>
+      </c>
+      <c r="D76">
+        <v>14</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>6863</v>
+      </c>
+      <c r="H76">
+        <v>44167</v>
+      </c>
+      <c r="I76">
+        <v>1.401E-2</v>
+      </c>
+      <c r="J76" t="s">
+        <v>13</v>
+      </c>
+      <c r="K76" t="s">
+        <v>28</v>
+      </c>
+      <c r="L76">
+        <v>4</v>
+      </c>
+      <c r="M76" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>0</v>
+      </c>
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="C77">
+        <v>14</v>
+      </c>
+      <c r="D77">
+        <v>14</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <v>15620</v>
+      </c>
+      <c r="H77">
+        <v>101576</v>
+      </c>
+      <c r="I77">
+        <v>2.9019E-2</v>
+      </c>
+      <c r="J77" t="s">
+        <v>13</v>
+      </c>
+      <c r="K77" t="s">
+        <v>29</v>
+      </c>
+      <c r="L77">
+        <v>5</v>
+      </c>
+      <c r="M77" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>0</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78">
+        <v>14</v>
+      </c>
+      <c r="D78">
+        <v>14</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>9943</v>
+      </c>
+      <c r="H78">
+        <v>73510</v>
+      </c>
+      <c r="I78">
+        <v>3.7025000000000002E-2</v>
+      </c>
+      <c r="J78" t="s">
+        <v>13</v>
+      </c>
+      <c r="K78" t="s">
+        <v>14</v>
+      </c>
+      <c r="L78">
+        <v>6</v>
+      </c>
+      <c r="M78" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>0</v>
+      </c>
+      <c r="B79">
+        <v>2</v>
+      </c>
+      <c r="C79">
+        <v>14</v>
+      </c>
+      <c r="D79">
+        <v>14</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <v>4266</v>
+      </c>
+      <c r="H79">
+        <v>48926</v>
+      </c>
+      <c r="I79">
+        <v>0.44729600000000003</v>
+      </c>
+      <c r="J79" t="s">
+        <v>13</v>
+      </c>
+      <c r="K79" t="s">
+        <v>16</v>
+      </c>
+      <c r="L79">
+        <v>7</v>
+      </c>
+      <c r="M79" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>0</v>
+      </c>
+      <c r="B80">
+        <v>2</v>
+      </c>
+      <c r="C80">
+        <v>14</v>
+      </c>
+      <c r="D80">
+        <v>14</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80">
+        <v>3941</v>
+      </c>
+      <c r="H80">
+        <v>37286</v>
+      </c>
+      <c r="I80">
+        <v>0.25316899999999998</v>
+      </c>
+      <c r="J80" t="s">
+        <v>13</v>
+      </c>
+      <c r="K80" t="s">
+        <v>17</v>
+      </c>
+      <c r="L80">
+        <v>8</v>
+      </c>
+      <c r="M80" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>0</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81">
+        <v>14</v>
+      </c>
+      <c r="D81">
+        <v>14</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81">
+        <v>1506</v>
+      </c>
+      <c r="H81">
+        <v>25600</v>
+      </c>
+      <c r="I81">
+        <v>1.016672</v>
+      </c>
+      <c r="J81" t="s">
+        <v>13</v>
+      </c>
+      <c r="K81" t="s">
+        <v>30</v>
+      </c>
+      <c r="L81">
+        <v>9</v>
+      </c>
+      <c r="M81" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>0</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82">
+        <v>14</v>
+      </c>
+      <c r="D82">
+        <v>14</v>
+      </c>
+      <c r="E82">
+        <v>2</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>4</v>
+      </c>
+      <c r="H82">
+        <v>1455</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82" t="s">
+        <v>13</v>
+      </c>
+      <c r="K82" t="s">
+        <v>31</v>
+      </c>
+      <c r="L82">
+        <v>10</v>
+      </c>
+      <c r="M82" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>0</v>
+      </c>
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83">
+        <v>14</v>
+      </c>
+      <c r="D83">
+        <v>14</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83">
+        <v>5</v>
+      </c>
+      <c r="H83">
+        <v>1518</v>
+      </c>
+      <c r="I83">
+        <v>5.0029999999999996E-3</v>
+      </c>
+      <c r="J83" t="s">
+        <v>13</v>
+      </c>
+      <c r="K83" t="s">
+        <v>32</v>
+      </c>
+      <c r="L83">
+        <v>11</v>
+      </c>
+      <c r="M83" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>0</v>
+      </c>
+      <c r="B84">
+        <v>2</v>
+      </c>
+      <c r="C84">
+        <v>14</v>
+      </c>
+      <c r="D84">
+        <v>14</v>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="F84">
+        <v>2</v>
+      </c>
+      <c r="G84">
+        <v>38627</v>
+      </c>
+      <c r="H84">
+        <v>619916</v>
+      </c>
+      <c r="I84">
+        <v>0.40927200000000002</v>
+      </c>
+      <c r="J84" t="s">
+        <v>13</v>
+      </c>
+      <c r="K84" t="s">
+        <v>24</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>0</v>
+      </c>
+      <c r="B85">
+        <v>2</v>
+      </c>
+      <c r="C85">
+        <v>14</v>
+      </c>
+      <c r="D85">
+        <v>14</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="F85">
+        <v>2</v>
+      </c>
+      <c r="G85">
+        <v>38399</v>
+      </c>
+      <c r="H85">
+        <v>469685</v>
+      </c>
+      <c r="I85">
+        <v>0.17411599999999999</v>
+      </c>
+      <c r="J85" t="s">
+        <v>13</v>
+      </c>
+      <c r="K85" t="s">
+        <v>25</v>
+      </c>
+      <c r="L85">
+        <v>1</v>
+      </c>
+      <c r="M85" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>0</v>
+      </c>
+      <c r="B86">
+        <v>2</v>
+      </c>
+      <c r="C86">
+        <v>14</v>
+      </c>
+      <c r="D86">
+        <v>14</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="F86">
+        <v>2</v>
+      </c>
+      <c r="G86">
+        <v>51437</v>
+      </c>
+      <c r="H86">
+        <v>399251</v>
+      </c>
+      <c r="I86">
+        <v>0.17211399999999999</v>
+      </c>
+      <c r="J86" t="s">
+        <v>13</v>
+      </c>
+      <c r="K86" t="s">
+        <v>26</v>
+      </c>
+      <c r="L86">
+        <v>2</v>
+      </c>
+      <c r="M86" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>0</v>
+      </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87">
+        <v>14</v>
+      </c>
+      <c r="D87">
+        <v>14</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+      <c r="F87">
+        <v>2</v>
+      </c>
+      <c r="G87">
+        <v>430416</v>
+      </c>
+      <c r="H87">
+        <v>3067008</v>
+      </c>
+      <c r="I87">
+        <v>0.88258499999999995</v>
+      </c>
+      <c r="J87" t="s">
+        <v>13</v>
+      </c>
+      <c r="K87" t="s">
+        <v>27</v>
+      </c>
+      <c r="L87">
+        <v>3</v>
+      </c>
+      <c r="M87" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>0</v>
+      </c>
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88">
+        <v>14</v>
+      </c>
+      <c r="D88">
+        <v>14</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="F88">
+        <v>2</v>
+      </c>
+      <c r="G88">
+        <v>99721</v>
+      </c>
+      <c r="H88">
+        <v>740711</v>
+      </c>
+      <c r="I88">
+        <v>0.235157</v>
+      </c>
+      <c r="J88" t="s">
+        <v>13</v>
+      </c>
+      <c r="K88" t="s">
+        <v>28</v>
+      </c>
+      <c r="L88">
+        <v>4</v>
+      </c>
+      <c r="M88" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>0</v>
+      </c>
+      <c r="B89">
+        <v>2</v>
+      </c>
+      <c r="C89">
+        <v>14</v>
+      </c>
+      <c r="D89">
+        <v>14</v>
+      </c>
+      <c r="E89">
+        <v>2</v>
+      </c>
+      <c r="F89">
+        <v>2</v>
+      </c>
+      <c r="G89">
+        <v>221515</v>
+      </c>
+      <c r="H89">
+        <v>1657116</v>
+      </c>
+      <c r="I89">
+        <v>0.463306</v>
+      </c>
+      <c r="J89" t="s">
+        <v>13</v>
+      </c>
+      <c r="K89" t="s">
+        <v>29</v>
+      </c>
+      <c r="L89">
+        <v>5</v>
+      </c>
+      <c r="M89" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>0</v>
+      </c>
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90">
+        <v>14</v>
+      </c>
+      <c r="D90">
+        <v>14</v>
+      </c>
+      <c r="E90">
+        <v>2</v>
+      </c>
+      <c r="F90">
+        <v>2</v>
+      </c>
+      <c r="G90">
+        <v>111419</v>
+      </c>
+      <c r="H90">
+        <v>1031176</v>
+      </c>
+      <c r="I90">
+        <v>0.54836300000000004</v>
+      </c>
+      <c r="J90" t="s">
+        <v>13</v>
+      </c>
+      <c r="K90" t="s">
+        <v>14</v>
+      </c>
+      <c r="L90">
+        <v>6</v>
+      </c>
+      <c r="M90" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>0</v>
+      </c>
+      <c r="B91">
+        <v>2</v>
+      </c>
+      <c r="C91">
+        <v>14</v>
+      </c>
+      <c r="D91">
+        <v>14</v>
+      </c>
+      <c r="E91">
+        <v>2</v>
+      </c>
+      <c r="F91">
+        <v>2</v>
+      </c>
+      <c r="G91">
+        <v>66737</v>
+      </c>
+      <c r="H91">
+        <v>801899</v>
+      </c>
+      <c r="I91">
+        <v>158.80049099999999</v>
+      </c>
+      <c r="J91" t="s">
+        <v>13</v>
+      </c>
+      <c r="K91" t="s">
+        <v>16</v>
+      </c>
+      <c r="L91">
+        <v>7</v>
+      </c>
+      <c r="M91" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>0</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92">
+        <v>14</v>
+      </c>
+      <c r="D92">
+        <v>14</v>
+      </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="F92">
+        <v>2</v>
+      </c>
+      <c r="G92">
+        <v>54764</v>
+      </c>
+      <c r="H92">
+        <v>560101</v>
+      </c>
+      <c r="I92">
+        <v>51.265925000000003</v>
+      </c>
+      <c r="J92" t="s">
+        <v>13</v>
+      </c>
+      <c r="K92" t="s">
+        <v>17</v>
+      </c>
+      <c r="L92">
+        <v>8</v>
+      </c>
+      <c r="M92" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="B93">
+        <v>2</v>
+      </c>
+      <c r="C93">
+        <v>14</v>
+      </c>
+      <c r="D93">
+        <v>14</v>
+      </c>
+      <c r="E93">
+        <v>2</v>
+      </c>
+      <c r="F93">
+        <v>2</v>
+      </c>
+      <c r="G93">
+        <v>20799</v>
+      </c>
+      <c r="H93">
+        <v>398376</v>
+      </c>
+      <c r="I93">
+        <v>195.367279</v>
+      </c>
+      <c r="J93" t="s">
+        <v>13</v>
+      </c>
+      <c r="K93" t="s">
+        <v>30</v>
+      </c>
+      <c r="L93">
+        <v>9</v>
+      </c>
+      <c r="M93" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>0</v>
+      </c>
+      <c r="B94">
+        <v>2</v>
+      </c>
+      <c r="C94">
+        <v>14</v>
+      </c>
+      <c r="D94">
+        <v>14</v>
+      </c>
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94">
+        <v>2</v>
+      </c>
+      <c r="G94">
+        <v>4</v>
+      </c>
+      <c r="H94">
+        <v>1455</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94" t="s">
+        <v>13</v>
+      </c>
+      <c r="K94" t="s">
+        <v>31</v>
+      </c>
+      <c r="L94">
+        <v>10</v>
+      </c>
+      <c r="M94" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>0</v>
+      </c>
+      <c r="B95">
+        <v>2</v>
+      </c>
+      <c r="C95">
+        <v>14</v>
+      </c>
+      <c r="D95">
+        <v>14</v>
+      </c>
+      <c r="E95">
+        <v>2</v>
+      </c>
+      <c r="F95">
+        <v>2</v>
+      </c>
+      <c r="G95">
+        <v>5</v>
+      </c>
+      <c r="H95">
+        <v>1518</v>
+      </c>
+      <c r="I95">
+        <v>6.0029999999999997E-3</v>
+      </c>
+      <c r="J95" t="s">
+        <v>13</v>
+      </c>
+      <c r="K95" t="s">
+        <v>32</v>
+      </c>
+      <c r="L95">
+        <v>11</v>
+      </c>
+      <c r="M95" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>